<commit_message>
Virtualization methods' files fixed
</commit_message>
<xml_diff>
--- a/6семестр/Методы Оптимизации и Исследования Операций/19Б12_Панюшин_14.xlsx
+++ b/6семестр/Методы Оптимизации и Исследования Операций/19Б12_Панюшин_14.xlsx
@@ -4,62 +4,65 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Отчет о результатах 1" sheetId="5" r:id="rId1"/>
-    <sheet name="Решение" sheetId="1" r:id="rId2"/>
+    <sheet name="Отчет о результатах 1" sheetId="6" r:id="rId1"/>
+    <sheet name="Отчет об устойчивости 1" sheetId="7" r:id="rId2"/>
+    <sheet name="Отчет о пределах 1" sheetId="8" r:id="rId3"/>
+    <sheet name="Решение" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">Решение!$B$17:$D$17</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Решение!$B$17:$D$17</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Решение!$B$17:$D$17</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Решение!$E$9:$E$10</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Решение!$D$17</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Решение!$E$9:$E$10</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Решение!$E$12</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">4</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">"целое"</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Решение!$B$19:$D$19</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Решение!$G$9:$G$10</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Решение!$G$9:$G$10</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Решение!$B$17:$D$17</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Решение!$B$17:$D$17</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Решение!$E$9:$E$10</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Решение!$E$9:$E$10</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">Решение!$D$17</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">Решение!$E$9:$E$10</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Решение!$E$12</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">Решение!$B$19:$D$19</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Решение!$G$9:$G$10</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">Решение!$G$9:$G$10</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">Решение!$G$9:$G$10</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>Ячейка</t>
   </si>
@@ -220,15 +223,6 @@
     <t>Без привязки</t>
   </si>
   <si>
-    <t>$B$17:$D$17=Целочисленное</t>
-  </si>
-  <si>
-    <t>Отчет создан: 08.03.2022 20:59:40</t>
-  </si>
-  <si>
-    <t>Время решения: 0 секунд.</t>
-  </si>
-  <si>
     <t>Максимальное время 100 с,  Число итераций 100, Precision 0,000001</t>
   </si>
   <si>
@@ -239,6 +233,75 @@
   </si>
   <si>
     <t>$D$17&gt;=$D$19</t>
+  </si>
+  <si>
+    <t>Отчет создан: 14.03.2022 20:46:16</t>
+  </si>
+  <si>
+    <t>Время решения: 0,016 секунд.</t>
+  </si>
+  <si>
+    <t>Продолжить</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 15.0 Отчет об устойчивости</t>
+  </si>
+  <si>
+    <t>Окончательное</t>
+  </si>
+  <si>
+    <t>Значение</t>
+  </si>
+  <si>
+    <t>Приведенн.</t>
+  </si>
+  <si>
+    <t>Стоимость</t>
+  </si>
+  <si>
+    <t>Целевая функция</t>
+  </si>
+  <si>
+    <t>Коэффициент</t>
+  </si>
+  <si>
+    <t>Допустимое</t>
+  </si>
+  <si>
+    <t>Увеличение</t>
+  </si>
+  <si>
+    <t>Уменьшение</t>
+  </si>
+  <si>
+    <t>Тень</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Ограничение</t>
+  </si>
+  <si>
+    <t>Правая сторона</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 15.0 Отчет о пределах</t>
+  </si>
+  <si>
+    <t>Переменная</t>
+  </si>
+  <si>
+    <t>Нижний</t>
+  </si>
+  <si>
+    <t>Предел</t>
+  </si>
+  <si>
+    <t>Результат</t>
+  </si>
+  <si>
+    <t>Верхний</t>
   </si>
 </sst>
 </file>
@@ -291,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -512,17 +575,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -556,9 +634,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -596,12 +671,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -906,16 +993,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
     <col min="3" max="3" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
@@ -935,7 +1020,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,7 +1042,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,7 +1058,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -987,30 +1072,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="29" t="s">
+      <c r="B15" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="32" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="28">
         <v>4560</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="28">
         <v>4560</v>
       </c>
     </row>
@@ -1020,71 +1105,71 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="29" t="s">
+      <c r="B20" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="32" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="29">
         <v>80</v>
       </c>
-      <c r="E21" s="32">
-        <v>80</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>39</v>
+      <c r="E21" s="29">
+        <v>79.999999999999929</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="29">
         <v>240</v>
       </c>
-      <c r="E22" s="32">
-        <v>240</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>39</v>
+      <c r="E22" s="29">
+        <v>240.00000000000006</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="31">
-        <v>0</v>
-      </c>
-      <c r="E23" s="31">
-        <v>0</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>39</v>
+      <c r="D23" s="28">
+        <v>0</v>
+      </c>
+      <c r="E23" s="28">
+        <v>0</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1093,134 +1178,124 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="29" t="s">
+      <c r="B27" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="29">
         <v>60</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="30">
+      <c r="G28" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="32">
-        <v>40</v>
-      </c>
-      <c r="E29" s="30" t="s">
+      <c r="D29" s="29">
+        <v>39.999999999999993</v>
+      </c>
+      <c r="E29" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="30">
+      <c r="G29" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="32">
-        <v>80</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="30" t="s">
+      <c r="D30" s="29">
+        <v>79.999999999999929</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="32">
-        <v>80</v>
+      <c r="G30" s="29">
+        <v>79.999999999999929</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="32">
-        <v>240</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="30" t="s">
+      <c r="D31" s="29">
+        <v>240.00000000000006</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G31" s="32">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="30" t="s">
+      <c r="G31" s="29">
+        <v>40.000000000000057</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="32">
-        <v>0</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" s="30" t="s">
+      <c r="D32" s="28">
+        <v>0</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
+      <c r="G32" s="28">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1229,240 +1304,671 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="27">
+        <v>79.999999999999929</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27">
+        <v>12</v>
+      </c>
+      <c r="G9" s="27">
+        <v>2.9999999999999947</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="27">
+        <v>240.00000000000006</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27">
+        <v>15</v>
+      </c>
+      <c r="G10" s="27">
+        <v>1</v>
+      </c>
+      <c r="H10" s="27">
+        <v>1.4999999999999976</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="26">
+        <v>0</v>
+      </c>
+      <c r="E11" s="26">
+        <v>-0.59999999999999909</v>
+      </c>
+      <c r="F11" s="26">
+        <v>3</v>
+      </c>
+      <c r="G11" s="26">
+        <v>0.59999999999999909</v>
+      </c>
+      <c r="H11" s="26">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="27">
+        <v>60</v>
+      </c>
+      <c r="E16" s="27">
+        <v>72</v>
+      </c>
+      <c r="F16" s="27">
+        <v>60</v>
+      </c>
+      <c r="G16" s="27">
+        <v>19.999999999999968</v>
+      </c>
+      <c r="H16" s="27">
+        <v>5.0000000000000062</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="26">
+        <v>39.999999999999993</v>
+      </c>
+      <c r="E17" s="26">
+        <v>6.0000000000000018</v>
+      </c>
+      <c r="F17" s="26">
+        <v>40</v>
+      </c>
+      <c r="G17" s="26">
+        <v>6.6666666666666741</v>
+      </c>
+      <c r="H17" s="26">
+        <v>9.9999999999999893</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="28">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="F11" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="29">
+        <v>79.999999999999929</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0</v>
+      </c>
+      <c r="G13" s="29">
+        <v>3600.0000000000009</v>
+      </c>
+      <c r="I13" s="29">
+        <v>80.000000000000242</v>
+      </c>
+      <c r="J13" s="29">
+        <v>4560.0000000000036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="29">
+        <v>240.00000000000006</v>
+      </c>
+      <c r="F14" s="29">
+        <v>200</v>
+      </c>
+      <c r="G14" s="29">
+        <v>3959.9999999999991</v>
+      </c>
+      <c r="I14" s="29">
+        <v>239.99999999999673</v>
+      </c>
+      <c r="J14" s="29">
+        <v>4559.99999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0</v>
+      </c>
+      <c r="G15" s="28">
+        <v>4560</v>
+      </c>
+      <c r="I15" s="28">
+        <v>0</v>
+      </c>
+      <c r="J15" s="28">
+        <v>4560</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="15" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="2"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>0.15</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.2</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>0.05</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f>SUMPRODUCT(B9:D9,B17:D17)</f>
         <v>60</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="24">
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>0.2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.1</v>
       </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
         <f>SUMPRODUCT(B10:D10,$B$17:$D$17)</f>
+        <v>39.999999999999993</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="25">
         <v>40</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="27">
-        <v>40</v>
-      </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="17" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>12</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>15</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>3</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f>SUMPRODUCT(B12:D12,B17:D17)</f>
         <v>4560</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="21">
-        <v>80</v>
-      </c>
-      <c r="C17" s="22">
-        <v>240</v>
-      </c>
-      <c r="D17" s="23">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="19">
+        <v>79.999999999999929</v>
+      </c>
+      <c r="C17" s="20">
+        <v>240.00000000000006</v>
+      </c>
+      <c r="D17" s="21">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="4">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
         <v>200</v>
       </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>